<commit_message>
Copyright & Provider Fix
</commit_message>
<xml_diff>
--- a/tools/excel/cisco/mappings/mapping-cisco-ccf-v3.0-to-pcidss-4_0.xlsx
+++ b/tools/excel/cisco/mappings/mapping-cisco-ccf-v3.0-to-pcidss-4_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\cisco\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925BE45C-4203-4369-84C6-7EC6810195F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA45AE80-BF19-41E5-BF9B-A854A7F3E1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2508" yWindow="648" windowWidth="17280" windowHeight="9420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3615" yWindow="-14205" windowWidth="20865" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7016" uniqueCount="4871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7015" uniqueCount="4872">
   <si>
     <t>type</t>
   </si>
@@ -15566,6 +15566,9 @@
 - Identification of anomalies or suspicious activity as it occurs.
 - Issuance of prompt alerts upon detection of suspicious activity or anomaly to responsible personnel.
 - Response to alerts in accordance with documented response procedures.</t>
+  </si>
+  <si>
+    <t>Cisco</t>
   </si>
 </sst>
 </file>
@@ -15907,7 +15910,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -15934,8 +15939,8 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="B3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -15975,7 +15980,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>4871</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -15983,7 +15988,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>4871</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -16099,7 +16104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E577"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+    <sheetView topLeftCell="A166" workbookViewId="0">
       <selection activeCell="B175" sqref="B175"/>
     </sheetView>
   </sheetViews>

</xml_diff>